<commit_message>
Start making hash and try connect to DB
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P-app_183\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF816A4A-220F-4701-A9A8-72C6FA47BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04367F77-4564-4A6A-B8AA-EDA4F0C91D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -136,6 +136,15 @@
   <si>
     <t>J'ai envoier le lien du Trello à CSR mais le voici : https://tinyurl.com/t5w95m7x</t>
   </si>
+  <si>
+    <t>discution convocation samedi avec CSR</t>
+  </si>
+  <si>
+    <t>Crée un code qui permet de hash un mdp grace à crypto-js</t>
+  </si>
+  <si>
+    <t>lien doc utilisée : https://www.npmjs.com/package/crypto-js</t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-CH,1]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +197,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -212,10 +229,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,8 +285,12 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -588,9 +610,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -655,7 +677,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.10416666666666666</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -809,6 +831,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>12</v>
+      </c>
       <c r="B12" s="9">
         <v>45373</v>
       </c>
@@ -824,18 +849,42 @@
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="15">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45401</v>
+      </c>
+      <c r="C13" s="23">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="A14" s="15">
+        <v>16</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45401</v>
+      </c>
+      <c r="C14" s="23">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
@@ -6539,35 +6588,18 @@
       <formula1>$I$2:$N$2</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F14" r:id="rId1" display="https://www.npmjs.com/package/crypto-js" xr:uid="{906AF64D-BADD-42B5-90CF-E6A2AD12ACFB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6790,26 +6822,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6826,4 +6859,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Make the jwt token  work
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P-app_183\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F99B6-56E3-4752-B4F8-4C18F9F7F264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462BB1BB-FDB2-47E6-BFE4-9F9E88388508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3990" yWindow="3270" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>J'ai avancer sur le nouveau backend, il me reste l'authentification et les test insomnia/postman a effectuer</t>
+  </si>
+  <si>
+    <t>J'ai du me remettre dans le projet. Ensuite j'ai avancer sur mon backend puis j'ai aidé adrian qui ne savait plus quoi faire pour le projet.</t>
+  </si>
+  <si>
+    <t>Après le passage de tiago il ma dis qu'il ne faut pas faire de mock n'y de model donc je repart à zero, j'ai dû comprendre la route de login déjà crée ensuite on a reçu nos bultin semestriel.</t>
+  </si>
+  <si>
+    <t>Je bloque sur la connection</t>
+  </si>
+  <si>
+    <t>Je me rend compte que je n'ai pas la bonne version ducoup j'ai chercher la bonne puis commencer a tester la conection</t>
+  </si>
+  <si>
+    <t>j'arrive enfin a démarrer via npm start j'ai des erreur de port mais je suis sur la bonne voie</t>
+  </si>
+  <si>
+    <t>Erreur de port réglée,ethan ma aidée a gérer mon erreur de tocken</t>
   </si>
 </sst>
 </file>
@@ -617,8 +635,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -683,7 +701,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.23402777777777778</v>
+        <v>0.29652777777777783</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -911,7 +929,12 @@
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="A16" s="15">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45401</v>
+      </c>
       <c r="C16" s="23">
         <v>2.7777777777777776E-2</v>
       </c>
@@ -924,65 +947,117 @@
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="A17" s="15">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="A18" s="15">
+        <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="str">
+      <c r="A19" s="15">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="str">
+      <c r="A20" s="15">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C20" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="str">
+      <c r="A21" s="15">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B21" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C21" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="str">
+      <c r="A22" s="15">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C22" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6623,26 +6698,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6865,26 +6920,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6901,4 +6957,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>